<commit_message>
All Services Implemented with Symmetric Key Authorization
</commit_message>
<xml_diff>
--- a/Status Update.xlsx
+++ b/Status Update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -127,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,23 +144,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF323130"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,17 +176,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -835,23 +818,58 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18.75">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="50" spans="2:2" ht="15.75">
-      <c r="B50" s="4"/>
-    </row>
-    <row r="51" spans="2:2" ht="15.75">
-      <c r="B51" s="4"/>
-    </row>
-    <row r="53" spans="2:2" ht="15.75">
-      <c r="B53" s="4"/>
-    </row>
-    <row r="54" spans="2:2" ht="15.75">
-      <c r="B54" s="5"/>
-    </row>
-    <row r="55" spans="2:2" ht="15.75">
-      <c r="B55" s="4"/>
+    <row r="49" spans="1:6">
+      <c r="A49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>44085</v>
+      </c>
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="F52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="F53" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75">
+      <c r="B55" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>